<commit_message>
Fixed issue with having one long row
</commit_message>
<xml_diff>
--- a/TestFileToImport.xlsx
+++ b/TestFileToImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Docs\code\ChristmasDrawingJava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1137DDA4-6212-4B29-900E-69FB54F14C21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B511DD60-FC53-4ED0-ACDD-974C9197803F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48A1F277-246F-4175-BF30-A984D4C5F475}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>Josh</t>
   </si>
@@ -403,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C689C9B-E282-44F0-8F8D-22D3814D5FC0}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -427,12 +427,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>